<commit_message>
updating code with correct discounting, option for cost breakdown in the main runner menu and cost breakdown summaries
</commit_message>
<xml_diff>
--- a/test_data/specs_mw_one_scenario.xlsx
+++ b/test_data/specs_mw_one_scenario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,6 +12,8 @@
     <sheet name="SpecsDataCalib" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="SpecsDataCalib1" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="SpecsDataCalib2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SpecsDataCalib3" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="SpecsDataCalib4" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -102,30 +104,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -404,15 +406,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="8"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="17"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="32.140625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="26"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="28"/>
-    <col customWidth="1" max="6" min="6" width="14.42578125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="10.85546875"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="22.140625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="20.42578125"/>
+    <col width="8" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="17" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="32.140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="26" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="28" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="14.42578125" customWidth="1" min="6" max="6"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="22.140625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -492,7 +494,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -510,14 +512,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="10.7109375"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="14.42578125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="17.28515625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="14.85546875"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="11"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" width="16.5703125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" width="19.5703125"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="14.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="11" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="19.5703125" bestFit="1" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -668,7 +670,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
@@ -687,38 +689,38 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="8"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="12.5703125"/>
-    <col customWidth="1" max="3" min="3" style="2" width="9.140625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="8.140625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="2" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="2" width="19.42578125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="2" width="12.28515625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="2" width="20"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="2" width="15.85546875"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="2" width="15.42578125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="2" width="18.5703125"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="2" width="22.140625"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="2" width="23"/>
-    <col bestFit="1" customWidth="1" max="14" min="14" style="2" width="26.85546875"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" style="2" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="16" min="16" style="2" width="11.5703125"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" style="2" width="20.42578125"/>
-    <col bestFit="1" customWidth="1" max="18" min="18" style="2" width="21.140625"/>
-    <col bestFit="1" customWidth="1" max="19" min="19" style="2" width="40.28515625"/>
-    <col bestFit="1" customWidth="1" max="20" min="20" style="2" width="10.140625"/>
-    <col bestFit="1" customWidth="1" max="21" min="21" style="2" width="15.5703125"/>
-    <col bestFit="1" customWidth="1" max="22" min="22" style="2" width="16.42578125"/>
-    <col bestFit="1" customWidth="1" max="23" min="23" style="2" width="13.42578125"/>
-    <col customWidth="1" max="24" min="24" style="2" width="12.140625"/>
-    <col customWidth="1" max="25" min="25" style="2" width="12.7109375"/>
-    <col bestFit="1" customWidth="1" max="26" min="26" style="2" width="14.7109375"/>
-    <col bestFit="1" customWidth="1" max="27" min="27" style="2" width="11.28515625"/>
-    <col bestFit="1" customWidth="1" max="28" min="28" style="2" width="12.140625"/>
-    <col bestFit="1" customWidth="1" max="29" min="29" style="2" width="12.7109375"/>
-    <col bestFit="1" customWidth="1" max="31" min="30" style="2" width="20"/>
-    <col customWidth="1" max="46" min="32" style="2" width="9.140625"/>
-    <col customWidth="1" max="16384" min="47" style="2" width="9.140625"/>
+    <col width="8" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="12.5703125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="9.140625" customWidth="1" style="2" min="3" max="3"/>
+    <col width="8.140625" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="12.5703125" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
+    <col width="12.28515625" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="20" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
+    <col width="15.85546875" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
+    <col width="15.42578125" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
+    <col width="22.140625" bestFit="1" customWidth="1" style="2" min="12" max="12"/>
+    <col width="23" bestFit="1" customWidth="1" style="2" min="13" max="13"/>
+    <col width="26.85546875" bestFit="1" customWidth="1" style="2" min="14" max="14"/>
+    <col width="10.5703125" bestFit="1" customWidth="1" style="2" min="15" max="15"/>
+    <col width="11.5703125" bestFit="1" customWidth="1" style="2" min="16" max="16"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" style="2" min="17" max="17"/>
+    <col width="21.140625" bestFit="1" customWidth="1" style="2" min="18" max="18"/>
+    <col width="40.28515625" bestFit="1" customWidth="1" style="2" min="19" max="19"/>
+    <col width="10.140625" bestFit="1" customWidth="1" style="2" min="20" max="20"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" style="2" min="21" max="21"/>
+    <col width="16.42578125" bestFit="1" customWidth="1" style="2" min="22" max="22"/>
+    <col width="13.42578125" bestFit="1" customWidth="1" style="2" min="23" max="23"/>
+    <col width="12.140625" customWidth="1" style="2" min="24" max="24"/>
+    <col width="12.7109375" customWidth="1" style="2" min="25" max="25"/>
+    <col width="14.7109375" bestFit="1" customWidth="1" style="2" min="26" max="26"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" style="2" min="27" max="27"/>
+    <col width="12.140625" bestFit="1" customWidth="1" style="2" min="28" max="28"/>
+    <col width="12.7109375" bestFit="1" customWidth="1" style="2" min="29" max="29"/>
+    <col width="20" bestFit="1" customWidth="1" style="2" min="30" max="31"/>
+    <col width="9.140625" customWidth="1" style="2" min="32" max="46"/>
+    <col width="9.140625" customWidth="1" style="2" min="47" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -966,7 +968,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1241,7 +1243,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1516,7 +1518,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1791,6 +1793,556 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>CountryCode</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>StartYear</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>EndYEar</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>PopStartYear</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>UrbanRatioStartYear</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>UrbanCutOff</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>UrbanRatioModelled</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
+        <is>
+          <t>PopEndYearHigh</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>PopEndYearLow</t>
+        </is>
+      </c>
+      <c r="K1" s="5" t="inlineStr">
+        <is>
+          <t>UrbanRatioEndYear</t>
+        </is>
+      </c>
+      <c r="L1" s="5" t="inlineStr">
+        <is>
+          <t>NumPeoplePerHHRural</t>
+        </is>
+      </c>
+      <c r="M1" s="5" t="inlineStr">
+        <is>
+          <t>NumPeoplePerHHUrban</t>
+        </is>
+      </c>
+      <c r="N1" s="5" t="inlineStr">
+        <is>
+          <t>GridCapacityInvestmentCost</t>
+        </is>
+      </c>
+      <c r="O1" s="5" t="inlineStr">
+        <is>
+          <t>GridLosses</t>
+        </is>
+      </c>
+      <c r="P1" s="5" t="inlineStr">
+        <is>
+          <t>BaseToPeak</t>
+        </is>
+      </c>
+      <c r="Q1" s="5" t="inlineStr">
+        <is>
+          <t>ExistingGridCostRatio</t>
+        </is>
+      </c>
+      <c r="R1" s="5" t="inlineStr">
+        <is>
+          <t>MaxGridExtensionDist</t>
+        </is>
+      </c>
+      <c r="S1" s="5" t="inlineStr">
+        <is>
+          <t>NewGridGenerationCapacityAnnualLimitMW</t>
+        </is>
+      </c>
+      <c r="T1" s="5" t="inlineStr">
+        <is>
+          <t>ElecActual</t>
+        </is>
+      </c>
+      <c r="U1" s="5" t="inlineStr">
+        <is>
+          <t>Rural_elec_ratio</t>
+        </is>
+      </c>
+      <c r="V1" s="5" t="inlineStr">
+        <is>
+          <t>Urban_elec_ratio</t>
+        </is>
+      </c>
+      <c r="W1" s="5" t="inlineStr">
+        <is>
+          <t>ElecModelled</t>
+        </is>
+      </c>
+      <c r="X1" s="5" t="inlineStr">
+        <is>
+          <t>urban_elec_ratio_modelled</t>
+        </is>
+      </c>
+      <c r="Y1" s="5" t="inlineStr">
+        <is>
+          <t>rural_elec_ratio_modelled</t>
+        </is>
+      </c>
+      <c r="Z1" s="5" t="inlineStr">
+        <is>
+          <t>MinNightLights</t>
+        </is>
+      </c>
+      <c r="AA1" s="5" t="inlineStr">
+        <is>
+          <t>DistToTrans</t>
+        </is>
+      </c>
+      <c r="AB1" s="5" t="inlineStr">
+        <is>
+          <t>MaxGridDist</t>
+        </is>
+      </c>
+      <c r="AC1" s="5" t="inlineStr">
+        <is>
+          <t>MaxRoadDist</t>
+        </is>
+      </c>
+      <c r="AD1" s="5" t="inlineStr">
+        <is>
+          <t>PopCutOffRoundOne</t>
+        </is>
+      </c>
+      <c r="AE1" s="5" t="inlineStr">
+        <is>
+          <t>PopCutOffRoundTwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Malawi</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>mw</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="E2" t="n">
+        <v>18620000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.1609394603523363</v>
+      </c>
+      <c r="I2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>26600000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1874</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>50</v>
+      </c>
+      <c r="S2" t="n">
+        <v>300</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.5104112205648693</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.0331974777603167</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>CountryCode</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>StartYear</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>EndYEar</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>PopStartYear</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>UrbanRatioStartYear</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>UrbanCutOff</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>UrbanRatioModelled</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
+        <is>
+          <t>PopEndYearHigh</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>PopEndYearLow</t>
+        </is>
+      </c>
+      <c r="K1" s="5" t="inlineStr">
+        <is>
+          <t>UrbanRatioEndYear</t>
+        </is>
+      </c>
+      <c r="L1" s="5" t="inlineStr">
+        <is>
+          <t>NumPeoplePerHHRural</t>
+        </is>
+      </c>
+      <c r="M1" s="5" t="inlineStr">
+        <is>
+          <t>NumPeoplePerHHUrban</t>
+        </is>
+      </c>
+      <c r="N1" s="5" t="inlineStr">
+        <is>
+          <t>GridCapacityInvestmentCost</t>
+        </is>
+      </c>
+      <c r="O1" s="5" t="inlineStr">
+        <is>
+          <t>GridLosses</t>
+        </is>
+      </c>
+      <c r="P1" s="5" t="inlineStr">
+        <is>
+          <t>BaseToPeak</t>
+        </is>
+      </c>
+      <c r="Q1" s="5" t="inlineStr">
+        <is>
+          <t>ExistingGridCostRatio</t>
+        </is>
+      </c>
+      <c r="R1" s="5" t="inlineStr">
+        <is>
+          <t>MaxGridExtensionDist</t>
+        </is>
+      </c>
+      <c r="S1" s="5" t="inlineStr">
+        <is>
+          <t>NewGridGenerationCapacityAnnualLimitMW</t>
+        </is>
+      </c>
+      <c r="T1" s="5" t="inlineStr">
+        <is>
+          <t>ElecActual</t>
+        </is>
+      </c>
+      <c r="U1" s="5" t="inlineStr">
+        <is>
+          <t>Rural_elec_ratio</t>
+        </is>
+      </c>
+      <c r="V1" s="5" t="inlineStr">
+        <is>
+          <t>Urban_elec_ratio</t>
+        </is>
+      </c>
+      <c r="W1" s="5" t="inlineStr">
+        <is>
+          <t>ElecModelled</t>
+        </is>
+      </c>
+      <c r="X1" s="5" t="inlineStr">
+        <is>
+          <t>urban_elec_ratio_modelled</t>
+        </is>
+      </c>
+      <c r="Y1" s="5" t="inlineStr">
+        <is>
+          <t>rural_elec_ratio_modelled</t>
+        </is>
+      </c>
+      <c r="Z1" s="5" t="inlineStr">
+        <is>
+          <t>MinNightLights</t>
+        </is>
+      </c>
+      <c r="AA1" s="5" t="inlineStr">
+        <is>
+          <t>DistToTrans</t>
+        </is>
+      </c>
+      <c r="AB1" s="5" t="inlineStr">
+        <is>
+          <t>MaxGridDist</t>
+        </is>
+      </c>
+      <c r="AC1" s="5" t="inlineStr">
+        <is>
+          <t>MaxRoadDist</t>
+        </is>
+      </c>
+      <c r="AD1" s="5" t="inlineStr">
+        <is>
+          <t>PopCutOffRoundOne</t>
+        </is>
+      </c>
+      <c r="AE1" s="5" t="inlineStr">
+        <is>
+          <t>PopCutOffRoundTwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Malawi</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>mw</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="E2" t="n">
+        <v>18620000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.1609394603523363</v>
+      </c>
+      <c r="I2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>26600000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1874</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>50</v>
+      </c>
+      <c r="S2" t="n">
+        <v>300</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.5104112205648693</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.0331974777603167</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>